<commit_message>
Add builder for data
</commit_message>
<xml_diff>
--- a/my.xlsx
+++ b/my.xlsx
@@ -508,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,6 +626,130 @@
       <c r="T2" s="6"/>
       <c r="U2" s="3"/>
     </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1">
+        <v>1</v>
+      </c>
+      <c r="P3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>1</v>
+      </c>
+      <c r="R3" s="1">
+        <v>1</v>
+      </c>
+      <c r="S3" s="1">
+        <v>1</v>
+      </c>
+      <c r="T3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1">
+        <v>7</v>
+      </c>
+      <c r="H4" s="1">
+        <v>8</v>
+      </c>
+      <c r="I4" s="1">
+        <v>9</v>
+      </c>
+      <c r="J4" s="1">
+        <v>10</v>
+      </c>
+      <c r="K4" s="1">
+        <v>11</v>
+      </c>
+      <c r="L4" s="1">
+        <v>12</v>
+      </c>
+      <c r="M4" s="1">
+        <v>13</v>
+      </c>
+      <c r="N4" s="1">
+        <v>14</v>
+      </c>
+      <c r="O4" s="1">
+        <v>15</v>
+      </c>
+      <c r="P4" s="1">
+        <v>16</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>17</v>
+      </c>
+      <c r="R4" s="1">
+        <v>18</v>
+      </c>
+      <c r="S4" s="1">
+        <v>19</v>
+      </c>
+      <c r="T4" s="1">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="R1:R2"/>

</xml_diff>

<commit_message>
Bug fix in class  DataProcessing metod priceHotWaterInKitchen
</commit_message>
<xml_diff>
--- a/my.xlsx
+++ b/my.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="mySheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>Месяц</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Сумма за холодную воду</t>
-  </si>
-  <si>
-    <t>Сумма за холодеую воду</t>
   </si>
   <si>
     <t>Суммарный воотвод</t>
@@ -511,7 +508,7 @@
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD5"/>
+      <selection activeCell="A3" sqref="A3:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,10 +560,10 @@
       <c r="N1" s="7"/>
       <c r="O1" s="8"/>
       <c r="P1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="R1" s="5" t="s">
         <v>4</v>
@@ -584,37 +581,37 @@
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="M2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
remove fields in xlsx
</commit_message>
<xml_diff>
--- a/my.xlsx
+++ b/my.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Test\Documents\Java_Projects\Price_For_Counters\"/>
     </mc:Choice>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>Месяц</t>
   </si>
@@ -67,16 +67,12 @@
   </si>
   <si>
     <t>Счетчик холодной воды текущие показания</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -509,32 +505,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="A4" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="10.0"/>
-    <col min="2" max="2" customWidth="true" style="1" width="11.42578125"/>
-    <col min="3" max="3" customWidth="true" style="1" width="17.140625"/>
-    <col min="4" max="4" customWidth="true" style="1" width="26.5703125"/>
-    <col min="5" max="6" customWidth="true" style="1" width="28.140625"/>
-    <col min="7" max="8" bestFit="true" customWidth="true" style="1" width="32.140625"/>
-    <col min="9" max="9" customWidth="true" style="1" width="16.0"/>
-    <col min="10" max="10" customWidth="true" style="1" width="26.85546875"/>
-    <col min="11" max="11" customWidth="true" style="1" width="25.0"/>
-    <col min="12" max="12" customWidth="true" style="1" width="17.7109375"/>
-    <col min="13" max="13" customWidth="true" style="1" width="29.42578125"/>
-    <col min="14" max="14" customWidth="true" style="1" width="21.42578125"/>
-    <col min="15" max="17" customWidth="true" style="1" width="15.28515625"/>
-    <col min="18" max="18" customWidth="true" style="1" width="18.5703125"/>
-    <col min="19" max="19" customWidth="true" style="1" width="16.5703125"/>
-    <col min="20" max="20" customWidth="true" style="1" width="16.28515625"/>
-    <col min="21" max="21" customWidth="true" style="1" width="18.140625"/>
-    <col min="22" max="16384" style="1" width="9.140625"/>
+    <col min="1" max="1" width="10" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="28.140625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="32.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16" style="1" customWidth="1"/>
+    <col min="10" max="10" width="26.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="25" style="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="29.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" style="1" customWidth="1"/>
+    <col min="15" max="17" width="15.28515625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="18.5703125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="16.5703125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="16.28515625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="18.140625" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -626,130 +622,6 @@
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
       <c r="U2" s="3"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="B3" t="s" s="1">
-        <v>16</v>
-      </c>
-      <c r="C3" t="n" s="1">
-        <v>754.49</v>
-      </c>
-      <c r="D3" t="n" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="E3" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="F3" t="n" s="1">
-        <v>243.16</v>
-      </c>
-      <c r="G3" t="n" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H3" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="I3" t="n" s="1">
-        <v>50.93</v>
-      </c>
-      <c r="J3" t="n" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="K3" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="L3" t="n" s="1">
-        <v>243.16</v>
-      </c>
-      <c r="M3" t="n" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="N3" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="O3" t="n" s="1">
-        <v>50.93</v>
-      </c>
-      <c r="P3" t="n" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="Q3" t="n" s="1">
-        <v>159.88</v>
-      </c>
-      <c r="R3" t="n" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="S3" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="T3" t="n" s="1">
-        <v>6.43</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="B4" t="s" s="1">
-        <v>16</v>
-      </c>
-      <c r="C4" t="n" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="D4" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="E4" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="F4" t="n" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="G4" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="H4" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="I4" t="n" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="J4" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="K4" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="L4" t="n" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="M4" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="N4" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="O4" t="n" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="P4" t="n" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="Q4" t="n" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="R4" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="S4" t="n" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="T4" t="n" s="1">
-        <v>0.0</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>